<commit_message>
Done results of experiment A, B, C
</commit_message>
<xml_diff>
--- a/Result.xlsx
+++ b/Result.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ProjectLapTrinh\Git\Classification-And-Clustering\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{700ACBA0-FEED-4FEB-97B8-41F524AB736D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F383AB70-22EB-4AFB-9A53-3EA59995DA15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{E8532C0F-116E-462F-AF90-AC43935B8C7C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E8532C0F-116E-462F-AF90-AC43935B8C7C}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="My Results" sheetId="2" r:id="rId1"/>
+    <sheet name="Results" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="22">
   <si>
     <t>Experiment Type</t>
   </si>
@@ -55,9 +56,6 @@
   </si>
   <si>
     <t>training set</t>
-  </si>
-  <si>
-    <t>validation</t>
   </si>
   <si>
     <t>percentage split</t>
@@ -65,17 +63,85 @@
   <si>
     <t>Augmented
 (preprocessed_hawks.csv)</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>cross validation</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">ID3 </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Lato"/>
+        <family val="2"/>
+      </rPr>
+      <t>(*)</t>
+    </r>
+  </si>
+  <si>
+    <t>(*) Sử dụng tập preprocessed_numeric2nominal_hawks.arff vì ID3 không chạy được với dữ liệu liên tục trong thí nghiệm này</t>
+  </si>
+  <si>
+    <t>Preprocessed
+(preprocessed_hawks.arff)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">B </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Lato"/>
+        <family val="2"/>
+      </rPr>
+      <t>(**)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">C </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Lato"/>
+        <family val="2"/>
+      </rPr>
+      <t>(***)</t>
+    </r>
+  </si>
+  <si>
+    <t>(**) thay đổi parameter của filter Discretize: attributeIndices = first-12; bins = 10</t>
+  </si>
+  <si>
+    <t>(***) thay đổi parameter của filter Discretize: attributeIndices = first-12; bins = 5; useEqualFrequency = true</t>
+  </si>
+  <si>
+    <t>avg of 10 x 10-fold cross validation</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="165" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="167" formatCode="0.0000%"/>
   </numFmts>
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -206,6 +272,21 @@
       <name val="Lato"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Lato"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="36">
     <fill>
@@ -419,7 +500,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -520,6 +601,43 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="6"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="6"/>
+      </top>
+      <bottom style="thin">
+        <color theme="6"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="6"/>
+      </top>
+      <bottom style="thin">
+        <color theme="6"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="6"/>
+      </right>
+      <top style="thin">
+        <color theme="6"/>
+      </top>
+      <bottom style="thin">
+        <color theme="6"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -640,36 +758,63 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="34" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="33" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="35" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="35" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="35" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="14" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="35" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="35" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="34" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="17" fillId="34" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="33" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="17" fillId="33" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="35" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="17" fillId="9" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="35" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="35" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="39">
@@ -1029,182 +1174,543 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{232B3B16-3102-4D4E-A189-B90944653FC6}">
-  <dimension ref="A1:K8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3AFD5B12-4BE9-4C24-8B96-2B844FA2388D}">
+  <dimension ref="A1:M11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:A5"/>
+      <selection activeCell="M9" sqref="M9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.44140625" customWidth="1"/>
-    <col min="2" max="2" width="19.33203125" customWidth="1"/>
-    <col min="3" max="11" width="10.77734375" customWidth="1"/>
+    <col min="1" max="1" width="24.42578125" customWidth="1"/>
+    <col min="2" max="2" width="19.28515625" customWidth="1"/>
+    <col min="3" max="4" width="10.7109375" customWidth="1"/>
+    <col min="5" max="5" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="10.7109375" customWidth="1"/>
+    <col min="8" max="8" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="11" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:13" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2" t="s">
+      <c r="B1" s="10"/>
+      <c r="C1" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2" t="s">
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1" s="10"/>
+      <c r="H1" s="10"/>
+      <c r="I1" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="J1" s="10"/>
+      <c r="K1" s="10"/>
+      <c r="L1" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="M1" s="10"/>
+    </row>
+    <row r="2" spans="1:13" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="13">
+        <v>0.98348000000000002</v>
+      </c>
+      <c r="D3" s="14">
+        <v>0.99229100000000003</v>
+      </c>
+      <c r="E3" s="15">
+        <v>1</v>
+      </c>
+      <c r="F3" s="13">
+        <v>0.98898699999999995</v>
+      </c>
+      <c r="G3" s="14">
+        <v>0.98458100000000004</v>
+      </c>
+      <c r="H3" s="15">
+        <v>1</v>
+      </c>
+      <c r="I3" s="13">
+        <v>0.97246699999999997</v>
+      </c>
+      <c r="J3" s="14">
+        <v>0.98348000000000002</v>
+      </c>
+      <c r="K3" s="15">
+        <v>0.99779700000000005</v>
+      </c>
+      <c r="L3" s="13"/>
+      <c r="M3" s="14"/>
+    </row>
+    <row r="4" spans="1:13" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="12"/>
+      <c r="B4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="13">
+        <v>0.98127799999999998</v>
+      </c>
+      <c r="D4" s="14">
+        <v>0.982379</v>
+      </c>
+      <c r="E4" s="15">
+        <v>0.80286299999999999</v>
+      </c>
+      <c r="F4" s="13">
+        <v>0.98788500000000001</v>
+      </c>
+      <c r="G4" s="14">
+        <v>0.97577100000000005</v>
+      </c>
+      <c r="H4" s="15">
+        <v>0.97136599999999995</v>
+      </c>
+      <c r="I4" s="13">
+        <v>0.969163</v>
+      </c>
+      <c r="J4" s="14">
+        <v>0.96806199999999998</v>
+      </c>
+      <c r="K4" s="15">
+        <v>0.96585900000000002</v>
+      </c>
+      <c r="L4" s="13"/>
+      <c r="M4" s="14"/>
+    </row>
+    <row r="5" spans="1:13" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="12"/>
+      <c r="B5" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="13">
+        <v>0.97734600000000005</v>
+      </c>
+      <c r="D5" s="14">
+        <v>0.98058299999999998</v>
+      </c>
+      <c r="E5" s="15">
+        <v>0.86084099999999997</v>
+      </c>
+      <c r="F5" s="13">
+        <v>0.98705500000000002</v>
+      </c>
+      <c r="G5" s="14">
+        <v>0.96440099999999995</v>
+      </c>
+      <c r="H5" s="15">
+        <v>0.983819</v>
+      </c>
+      <c r="I5" s="13">
+        <v>0.95792900000000003</v>
+      </c>
+      <c r="J5" s="14">
+        <v>0.967638</v>
+      </c>
+      <c r="K5" s="15">
+        <v>0.97087400000000001</v>
+      </c>
+      <c r="L5" s="13"/>
+      <c r="M5" s="14"/>
+    </row>
+    <row r="6" spans="1:13" ht="18" x14ac:dyDescent="0.25">
+      <c r="I6" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="J6" s="17"/>
+      <c r="K6" s="18"/>
+      <c r="L6" s="13"/>
+      <c r="M6" s="14"/>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9" s="7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10" s="7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A11" s="7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="7">
+    <mergeCell ref="L1:M1"/>
+    <mergeCell ref="I6:K6"/>
+    <mergeCell ref="A3:A5"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="C1:E1"/>
+    <mergeCell ref="F1:H1"/>
+    <mergeCell ref="I1:K1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{232B3B16-3102-4D4E-A189-B90944653FC6}">
+  <dimension ref="A1:N8"/>
+  <sheetViews>
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="A22" sqref="A22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="24.42578125" customWidth="1"/>
+    <col min="2" max="2" width="19.28515625" customWidth="1"/>
+    <col min="3" max="11" width="10.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2" t="s">
+      <c r="G1" s="10"/>
+      <c r="H1" s="10"/>
+      <c r="I1" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
+      <c r="J1" s="10"/>
+      <c r="K1" s="10"/>
+      <c r="L1" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="M1" s="10"/>
+      <c r="N1" s="10"/>
     </row>
-    <row r="2" spans="1:11" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="7" t="s">
+    <row r="2" spans="1:14" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="G2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="H2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="I2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="J2" s="3" t="s">
+      <c r="J2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="K2" s="3" t="s">
+      <c r="K2" s="2" t="s">
         <v>8</v>
       </c>
+      <c r="L2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="N2" s="2"/>
     </row>
-    <row r="3" spans="1:11" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="B3" s="4" t="s">
+    <row r="3" spans="1:14" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="5">
+      <c r="C3" s="4">
         <v>98.347999999999999</v>
       </c>
-      <c r="D3" s="6">
+      <c r="D3" s="5">
         <v>99.339200000000005</v>
       </c>
       <c r="E3" s="1">
         <v>100</v>
       </c>
-      <c r="F3" s="5">
+      <c r="F3" s="4">
         <v>98.898700000000005</v>
       </c>
-      <c r="G3" s="6">
+      <c r="G3" s="5">
         <v>98.898700000000005</v>
       </c>
       <c r="H3" s="1">
         <v>100</v>
       </c>
-      <c r="I3" s="5">
+      <c r="I3" s="4">
         <v>98.898700000000005</v>
       </c>
-      <c r="J3" s="6">
+      <c r="J3" s="5">
         <v>95.458100000000002</v>
       </c>
       <c r="K3" s="1">
         <v>100</v>
       </c>
+      <c r="L3" s="4"/>
+      <c r="M3" s="5"/>
+      <c r="N3" s="1"/>
     </row>
-    <row r="4" spans="1:11" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="8"/>
-      <c r="B4" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" s="5">
+    <row r="4" spans="1:14" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="9"/>
+      <c r="B4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="4">
         <v>98.237899999999996</v>
       </c>
-      <c r="D4" s="6">
+      <c r="D4" s="5">
         <v>95.458100000000002</v>
       </c>
       <c r="E4" s="1">
         <v>0.2203</v>
       </c>
-      <c r="F4" s="5">
+      <c r="F4" s="4">
         <v>99.898700000000005</v>
       </c>
-      <c r="G4" s="6">
+      <c r="G4" s="5">
         <v>99.898700000000005</v>
       </c>
       <c r="H4" s="1">
         <v>0.2203</v>
       </c>
-      <c r="I4" s="5">
+      <c r="I4" s="4">
         <v>99.898700000000005</v>
       </c>
-      <c r="J4" s="6">
+      <c r="J4" s="5">
         <v>97.466999999999999</v>
       </c>
       <c r="K4" s="1">
         <v>0.2203</v>
       </c>
+      <c r="L4" s="4"/>
+      <c r="M4" s="5"/>
+      <c r="N4" s="1"/>
     </row>
-    <row r="5" spans="1:11" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="8"/>
-      <c r="B5" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" s="5">
+    <row r="5" spans="1:14" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="9"/>
+      <c r="B5" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="4">
         <v>97.7346</v>
       </c>
-      <c r="D5" s="6">
+      <c r="D5" s="5">
         <v>96.116500000000002</v>
       </c>
       <c r="E5" s="1">
         <v>0</v>
       </c>
-      <c r="F5" s="5">
+      <c r="F5" s="4">
         <v>98.707499999999996</v>
       </c>
-      <c r="G5" s="6">
+      <c r="G5" s="5">
         <v>98.707499999999996</v>
       </c>
       <c r="H5" s="1">
         <v>0</v>
       </c>
-      <c r="I5" s="5">
+      <c r="I5" s="4">
         <v>98.707499999999996</v>
       </c>
-      <c r="J5" s="6">
+      <c r="J5" s="5">
         <v>96.440100000000001</v>
       </c>
       <c r="K5" s="1">
         <v>0</v>
       </c>
+      <c r="L5" s="4"/>
+      <c r="M5" s="5"/>
+      <c r="N5" s="1"/>
     </row>
-    <row r="6" spans="1:11" ht="19.95" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="7" spans="1:11" ht="19.95" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="8" spans="1:11" ht="19.95" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="6" spans="1:14" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="4">
+        <v>98.347999999999999</v>
+      </c>
+      <c r="D6" s="5">
+        <v>99.339200000000005</v>
+      </c>
+      <c r="E6" s="1">
+        <v>100</v>
+      </c>
+      <c r="F6" s="4">
+        <v>98.898700000000005</v>
+      </c>
+      <c r="G6" s="5">
+        <v>98.898700000000005</v>
+      </c>
+      <c r="H6" s="1">
+        <v>100</v>
+      </c>
+      <c r="I6" s="4">
+        <v>98.898700000000005</v>
+      </c>
+      <c r="J6" s="5">
+        <v>95.458100000000002</v>
+      </c>
+      <c r="K6" s="1">
+        <v>100</v>
+      </c>
+      <c r="L6" s="4"/>
+      <c r="M6" s="5"/>
+      <c r="N6" s="1"/>
+    </row>
+    <row r="7" spans="1:14" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="9"/>
+      <c r="B7" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="4">
+        <v>98.237899999999996</v>
+      </c>
+      <c r="D7" s="5">
+        <v>95.458100000000002</v>
+      </c>
+      <c r="E7" s="1">
+        <v>0.2203</v>
+      </c>
+      <c r="F7" s="4">
+        <v>99.898700000000005</v>
+      </c>
+      <c r="G7" s="5">
+        <v>99.898700000000005</v>
+      </c>
+      <c r="H7" s="1">
+        <v>0.2203</v>
+      </c>
+      <c r="I7" s="4">
+        <v>99.898700000000005</v>
+      </c>
+      <c r="J7" s="5">
+        <v>97.466999999999999</v>
+      </c>
+      <c r="K7" s="1">
+        <v>0.2203</v>
+      </c>
+      <c r="L7" s="4"/>
+      <c r="M7" s="5"/>
+      <c r="N7" s="1"/>
+    </row>
+    <row r="8" spans="1:14" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="9"/>
+      <c r="B8" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" s="4">
+        <v>97.7346</v>
+      </c>
+      <c r="D8" s="5">
+        <v>96.116500000000002</v>
+      </c>
+      <c r="E8" s="1">
+        <v>0</v>
+      </c>
+      <c r="F8" s="4">
+        <v>98.707499999999996</v>
+      </c>
+      <c r="G8" s="5">
+        <v>98.707499999999996</v>
+      </c>
+      <c r="H8" s="1">
+        <v>0</v>
+      </c>
+      <c r="I8" s="4">
+        <v>98.707499999999996</v>
+      </c>
+      <c r="J8" s="5">
+        <v>96.440100000000001</v>
+      </c>
+      <c r="K8" s="1">
+        <v>0</v>
+      </c>
+      <c r="L8" s="4"/>
+      <c r="M8" s="5"/>
+      <c r="N8" s="1"/>
+    </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="7">
+    <mergeCell ref="A6:A8"/>
+    <mergeCell ref="L1:N1"/>
     <mergeCell ref="C1:E1"/>
     <mergeCell ref="F1:H1"/>
     <mergeCell ref="I1:K1"/>

</xml_diff>